<commit_message>
change retroplanning + add team.txt
</commit_message>
<xml_diff>
--- a/00_Project Management/Retroplanning.xlsx
+++ b/00_Project Management/Retroplanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://campusdulac-my.sharepoint.com/personal/jonathan_dupau_campusdulac_com/Documents/Bureau/00_HACKATON/00_Project Management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D85A76A-AF86-4726-9947-42E95AE5A79C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{7D85A76A-AF86-4726-9947-42E95AE5A79C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{38647DB3-0CC9-4FA9-BBAB-22AAD15D38BC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
   <si>
     <t>Rétro Planning</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>maquette</t>
-  </si>
-  <si>
-    <t>logo</t>
   </si>
   <si>
     <t>livraison</t>
@@ -245,9 +242,6 @@
     </r>
   </si>
   <si>
-    <t>charte graphique ?????????</t>
-  </si>
-  <si>
     <t>CDC:                        ??????</t>
   </si>
   <si>
@@ -279,6 +273,30 @@
   </si>
   <si>
     <t>Réunion stand up 10" journalière</t>
+  </si>
+  <si>
+    <t>PORTFOLIO DEV</t>
+  </si>
+  <si>
+    <t>PORTFOLIO DESIGN</t>
+  </si>
+  <si>
+    <t>PORTFOLIO CHEF PROJET WEB</t>
+  </si>
+  <si>
+    <t>PORTFOLIO GRAPHISTE</t>
+  </si>
+  <si>
+    <t>CONTACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Design</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  dev</t>
+  </si>
+  <si>
+    <t>MENTION LEGAL / CGU</t>
   </si>
 </sst>
 </file>
@@ -1322,52 +1340,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1393,9 +1365,6 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1453,11 +1422,8 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1468,6 +1434,58 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1791,12 +1809,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R1004"/>
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="O9" sqref="O9"/>
+      <selection pane="topRight" activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1814,841 +1832,856 @@
     <col min="16" max="16" width="3.109375" customWidth="1"/>
     <col min="17" max="17" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="2.88671875" customWidth="1"/>
+    <col min="20" max="20" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="22.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:26" ht="22.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="80" t="s">
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="81"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-    </row>
-    <row r="2" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="V1" s="62"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="63"/>
+    </row>
+    <row r="2" spans="1:26" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="67"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="57"/>
+    </row>
+    <row r="3" spans="1:26" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
-      <c r="F2" s="77"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="75" t="s">
-        <v>38</v>
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="57" t="s">
+        <v>1</v>
       </c>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="75"/>
-    </row>
-    <row r="3" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="106" t="s">
+      <c r="L3" s="57"/>
+      <c r="M3" s="57"/>
+      <c r="N3" s="57"/>
+      <c r="O3" s="57"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="62" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="91"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="89"/>
+      <c r="I4" s="89"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="57" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="59"/>
+    </row>
+    <row r="5" spans="1:26" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="75" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="78"/>
-    </row>
-    <row r="4" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="106"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="77"/>
-      <c r="F4" s="77"/>
-      <c r="G4" s="78"/>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="78"/>
-      <c r="K4" s="75" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
-      <c r="P4" s="83"/>
-      <c r="Q4" s="83"/>
-      <c r="R4" s="77"/>
-    </row>
-    <row r="5" spans="1:18" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="78"/>
-      <c r="I5" s="78"/>
-      <c r="J5" s="78"/>
-      <c r="K5" s="78"/>
-      <c r="L5" s="78"/>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78"/>
-      <c r="O5" s="78"/>
-      <c r="P5" s="78"/>
-      <c r="Q5" s="78"/>
-      <c r="R5" s="78"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
+      <c r="R5" s="60"/>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="85"/>
-      <c r="G6" s="85"/>
-      <c r="H6" s="85"/>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="85"/>
-      <c r="M6" s="85"/>
-      <c r="N6" s="85"/>
-      <c r="O6" s="85"/>
-      <c r="P6" s="85"/>
-      <c r="Q6" s="85"/>
-      <c r="R6" s="85"/>
-    </row>
-    <row r="7" spans="1:18" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
+    </row>
+    <row r="7" spans="1:26" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="91" t="s">
+      <c r="D7" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="79"/>
-      <c r="M7" s="79"/>
-      <c r="N7" s="79"/>
-      <c r="O7" s="79"/>
-      <c r="P7" s="79"/>
-      <c r="Q7" s="79"/>
-      <c r="R7" s="79"/>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="93">
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="61"/>
+      <c r="R7" s="61"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="93"/>
+      <c r="B8" s="93"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="74">
         <v>15</v>
       </c>
-      <c r="E8" s="94">
+      <c r="E8" s="75">
         <v>16</v>
       </c>
-      <c r="F8" s="94">
+      <c r="F8" s="75">
         <v>17</v>
       </c>
-      <c r="G8" s="94">
+      <c r="G8" s="75">
         <v>18</v>
       </c>
-      <c r="H8" s="95">
+      <c r="H8" s="76">
         <v>19</v>
       </c>
-      <c r="I8" s="94">
+      <c r="I8" s="75">
         <v>6</v>
       </c>
-      <c r="J8" s="94">
+      <c r="J8" s="75">
         <v>7</v>
       </c>
-      <c r="K8" s="90"/>
-      <c r="L8" s="74"/>
-      <c r="M8" s="74"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="74"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="74"/>
-      <c r="R8" s="74"/>
-    </row>
-    <row r="9" spans="1:18" s="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="71"/>
+      <c r="L8" s="56"/>
+      <c r="M8" s="56"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="56"/>
+      <c r="Q8" s="56"/>
+      <c r="R8" s="56"/>
+    </row>
+    <row r="9" spans="1:26" s="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="48"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="74"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="74"/>
-    </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="56"/>
+      <c r="M9" s="56"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="56"/>
+      <c r="Q9" s="56"/>
+      <c r="R9" s="56"/>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C10" s="51"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="90"/>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="74"/>
-      <c r="P10" s="74"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="74"/>
-    </row>
-    <row r="11" spans="1:18" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="56"/>
+      <c r="R10" s="56"/>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B11" s="50"/>
       <c r="C11" s="51"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="97"/>
-      <c r="J11" s="97"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74"/>
-      <c r="O11" s="74"/>
-      <c r="P11" s="74"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-    </row>
-    <row r="12" spans="1:18" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="56"/>
+      <c r="R11" s="56"/>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="51"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="97"/>
-      <c r="J12" s="97"/>
-      <c r="K12" s="90"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="79"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="56"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="56"/>
+      <c r="R12" s="56"/>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="50"/>
       <c r="C13" s="51"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="98"/>
-      <c r="I13" s="97"/>
-      <c r="J13" s="97"/>
-      <c r="K13" s="90"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="74"/>
-      <c r="N13" s="74"/>
-      <c r="O13" s="74"/>
-      <c r="P13" s="74"/>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="74"/>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="56"/>
+      <c r="R13" s="56"/>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="50"/>
       <c r="C14" s="51"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98"/>
-      <c r="H14" s="98"/>
-      <c r="I14" s="97"/>
-      <c r="J14" s="97"/>
-      <c r="K14" s="90"/>
-      <c r="L14" s="74"/>
-      <c r="M14" s="74"/>
-      <c r="N14" s="74"/>
-      <c r="O14" s="74"/>
-      <c r="P14" s="74"/>
-      <c r="Q14" s="74"/>
-      <c r="R14" s="74"/>
-    </row>
-    <row r="15" spans="1:18" s="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="56"/>
+      <c r="R14" s="56"/>
+    </row>
+    <row r="15" spans="1:26" s="55" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="47"/>
       <c r="C15" s="48"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="94"/>
-      <c r="G15" s="94"/>
-      <c r="H15" s="94"/>
-      <c r="I15" s="97"/>
-      <c r="J15" s="97"/>
-      <c r="K15" s="90"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="74"/>
-      <c r="N15" s="74"/>
-      <c r="O15" s="74"/>
-      <c r="P15" s="74"/>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="74"/>
-    </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="78"/>
+      <c r="J15" s="78"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="56"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="56"/>
+      <c r="R15" s="56"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" s="51"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98"/>
-      <c r="H16" s="98"/>
-      <c r="I16" s="97"/>
-      <c r="J16" s="97"/>
-      <c r="K16" s="90"/>
-      <c r="L16" s="74"/>
-      <c r="M16" s="74"/>
-      <c r="N16" s="74"/>
-      <c r="O16" s="74"/>
-      <c r="P16" s="74"/>
-      <c r="Q16" s="74"/>
-      <c r="R16" s="74"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="82"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="78"/>
+      <c r="J16" s="78"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="56"/>
     </row>
     <row r="17" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="51"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="79"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="79"/>
+      <c r="I17" s="78"/>
+      <c r="J17" s="78"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+    </row>
+    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="51"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="78"/>
+      <c r="J18" s="78"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="56"/>
+      <c r="P18" s="56"/>
+      <c r="Q18" s="56"/>
+      <c r="R18" s="56"/>
+    </row>
+    <row r="19" spans="1:18" s="55" customFormat="1" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="75"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="78"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="56"/>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="56"/>
+      <c r="R19" s="56"/>
+    </row>
+    <row r="20" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="53"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="84"/>
+      <c r="F20" s="79"/>
+      <c r="G20" s="79"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="56"/>
+      <c r="R20" s="56"/>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="53"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="79"/>
+      <c r="E21" s="79"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="79"/>
+      <c r="H21" s="79"/>
+      <c r="I21" s="78"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="56"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="56"/>
+      <c r="R21" s="56"/>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="53"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="79"/>
+      <c r="E22" s="79"/>
+      <c r="F22" s="79"/>
+      <c r="G22" s="79"/>
+      <c r="H22" s="79"/>
+      <c r="I22" s="78"/>
+      <c r="J22" s="78"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="56"/>
+      <c r="P22" s="56"/>
+      <c r="Q22" s="56"/>
+      <c r="R22" s="56"/>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="53"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="78"/>
+      <c r="J23" s="78"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="56"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="56"/>
+      <c r="R23" s="56"/>
+    </row>
+    <row r="24" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="53"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
+      <c r="I24" s="78"/>
+      <c r="J24" s="78"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="56"/>
+      <c r="P24" s="56"/>
+      <c r="Q24" s="56"/>
+      <c r="R24" s="56"/>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="53"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="84"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
+      <c r="I25" s="78"/>
+      <c r="J25" s="78"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="56"/>
+      <c r="Q25" s="56"/>
+      <c r="R25" s="56"/>
+    </row>
+    <row r="26" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="53"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="79"/>
+      <c r="H26" s="79"/>
+      <c r="I26" s="78"/>
+      <c r="J26" s="78"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="P26" s="56"/>
+      <c r="Q26" s="56"/>
+      <c r="R26" s="56"/>
+    </row>
+    <row r="27" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="100"/>
-      <c r="E17" s="100"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="100"/>
-      <c r="H17" s="98"/>
-      <c r="I17" s="97"/>
-      <c r="J17" s="97"/>
-      <c r="K17" s="90"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="74"/>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
-    </row>
-    <row r="18" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="98"/>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="97"/>
-      <c r="J18" s="97"/>
-      <c r="K18" s="90"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="74"/>
-      <c r="N18" s="74"/>
-      <c r="O18" s="74"/>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="74"/>
-      <c r="R18" s="74"/>
-    </row>
-    <row r="19" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="54" t="s">
+      <c r="C27" s="51"/>
+      <c r="D27" s="79"/>
+      <c r="E27" s="79"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="79"/>
+      <c r="H27" s="79"/>
+      <c r="I27" s="78"/>
+      <c r="J27" s="78"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="56"/>
+      <c r="R27" s="56"/>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="53" t="s">
-        <v>41</v>
+      <c r="B28" s="53" t="s">
+        <v>40</v>
       </c>
-      <c r="C19" s="51"/>
-      <c r="D19" s="100"/>
-      <c r="E19" s="98"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="98"/>
-      <c r="I19" s="97"/>
-      <c r="J19" s="97"/>
-      <c r="K19" s="90"/>
-      <c r="L19" s="74"/>
-      <c r="M19" s="74"/>
-      <c r="N19" s="74"/>
-      <c r="O19" s="74"/>
-      <c r="P19" s="74"/>
-      <c r="Q19" s="74"/>
-      <c r="R19" s="74"/>
-    </row>
-    <row r="20" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="54" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="51"/>
-      <c r="D20" s="102"/>
-      <c r="E20" s="98"/>
-      <c r="F20" s="98"/>
-      <c r="G20" s="102"/>
-      <c r="H20" s="98"/>
-      <c r="I20" s="97"/>
-      <c r="J20" s="97"/>
-      <c r="K20" s="90"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="74"/>
-      <c r="P20" s="74"/>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="74"/>
-    </row>
-    <row r="21" spans="1:18" s="55" customFormat="1" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="48"/>
-      <c r="C21" s="48"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="94"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="94"/>
-      <c r="H21" s="94"/>
-      <c r="I21" s="97"/>
-      <c r="J21" s="97"/>
-      <c r="K21" s="90"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="74"/>
-      <c r="P21" s="74"/>
-      <c r="Q21" s="74"/>
-      <c r="R21" s="74"/>
-    </row>
-    <row r="22" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="98"/>
-      <c r="E22" s="98"/>
-      <c r="F22" s="98"/>
-      <c r="G22" s="98"/>
-      <c r="H22" s="98"/>
-      <c r="I22" s="97"/>
-      <c r="J22" s="97"/>
-      <c r="K22" s="90"/>
-      <c r="L22" s="74"/>
-      <c r="M22" s="74"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="74"/>
-      <c r="P22" s="74"/>
-      <c r="Q22" s="74"/>
-      <c r="R22" s="74"/>
-    </row>
-    <row r="23" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="49"/>
-      <c r="B23" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="98"/>
-      <c r="F23" s="98"/>
-      <c r="G23" s="98"/>
-      <c r="H23" s="98"/>
-      <c r="I23" s="97"/>
-      <c r="J23" s="97"/>
-      <c r="K23" s="90"/>
-      <c r="L23" s="74"/>
-      <c r="M23" s="74"/>
-      <c r="N23" s="74"/>
-      <c r="O23" s="74"/>
-      <c r="P23" s="74"/>
-      <c r="Q23" s="74"/>
-      <c r="R23" s="74"/>
-    </row>
-    <row r="24" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="49"/>
-      <c r="B24" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98"/>
-      <c r="H24" s="98"/>
-      <c r="I24" s="97"/>
-      <c r="J24" s="97"/>
-      <c r="K24" s="90"/>
-      <c r="L24" s="74"/>
-      <c r="M24" s="74"/>
-      <c r="N24" s="74"/>
-      <c r="O24" s="74"/>
-      <c r="P24" s="74"/>
-      <c r="Q24" s="74"/>
-      <c r="R24" s="74"/>
-    </row>
-    <row r="25" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="C28" s="51"/>
+      <c r="D28" s="79"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="78"/>
+      <c r="J28" s="78"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+    </row>
+    <row r="29" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="98"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="97"/>
-      <c r="J25" s="97"/>
-      <c r="K25" s="90"/>
-      <c r="L25" s="74"/>
-      <c r="M25" s="74"/>
-      <c r="N25" s="74"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="74"/>
-      <c r="R25" s="74"/>
-    </row>
-    <row r="26" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="98"/>
-      <c r="E26" s="98"/>
-      <c r="F26" s="98"/>
-      <c r="G26" s="104"/>
-      <c r="H26" s="104"/>
-      <c r="I26" s="97"/>
-      <c r="J26" s="97"/>
-      <c r="K26" s="90"/>
-      <c r="L26" s="74"/>
-      <c r="M26" s="74"/>
-      <c r="N26" s="74"/>
-      <c r="O26" s="74"/>
-      <c r="P26" s="74"/>
-      <c r="Q26" s="74"/>
-      <c r="R26" s="74"/>
-    </row>
-    <row r="27" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="98"/>
-      <c r="F27" s="98"/>
-      <c r="G27" s="103"/>
-      <c r="H27" s="103"/>
-      <c r="I27" s="97"/>
-      <c r="J27" s="97"/>
-      <c r="K27" s="90"/>
-      <c r="L27" s="74"/>
-      <c r="M27" s="74"/>
-      <c r="N27" s="74"/>
-      <c r="O27" s="74"/>
-      <c r="P27" s="74"/>
-      <c r="Q27" s="74"/>
-      <c r="R27" s="74"/>
-    </row>
-    <row r="28" spans="1:18" s="55" customFormat="1" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="94"/>
-      <c r="E28" s="94"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="94"/>
-      <c r="I28" s="97"/>
-      <c r="J28" s="97"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="74"/>
-      <c r="M28" s="74"/>
-      <c r="N28" s="74"/>
-      <c r="O28" s="74"/>
-      <c r="P28" s="74"/>
-      <c r="Q28" s="74"/>
-      <c r="R28" s="74"/>
-    </row>
-    <row r="29" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="s">
+      <c r="B29" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="53" t="s">
-        <v>42</v>
+      <c r="C29" s="51"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="84"/>
+      <c r="H29" s="84"/>
+      <c r="I29" s="78"/>
+      <c r="J29" s="78"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="56"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="56"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
+    </row>
+    <row r="30" spans="1:18" s="55" customFormat="1" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="47" t="s">
+        <v>37</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="98"/>
-      <c r="F29" s="98"/>
-      <c r="G29" s="104"/>
-      <c r="H29" s="104"/>
-      <c r="I29" s="97"/>
-      <c r="J29" s="97"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="74"/>
-      <c r="M29" s="74"/>
-      <c r="N29" s="74"/>
-      <c r="O29" s="74"/>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="74"/>
-      <c r="R29" s="74"/>
-    </row>
-    <row r="30" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="88"/>
-      <c r="L30" s="88"/>
-      <c r="M30" s="88"/>
-      <c r="N30" s="88"/>
-      <c r="O30" s="88"/>
-      <c r="P30" s="88"/>
-      <c r="Q30" s="88"/>
-      <c r="R30" s="88"/>
-    </row>
-    <row r="31" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="44"/>
-      <c r="P31" s="44"/>
-      <c r="Q31" s="44"/>
-      <c r="R31" s="44"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="78"/>
+      <c r="J30" s="78"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="56"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="56"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="56"/>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="51"/>
+      <c r="D31" s="79"/>
+      <c r="E31" s="79"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="85"/>
+      <c r="H31" s="85"/>
+      <c r="I31" s="78"/>
+      <c r="J31" s="78"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="56"/>
     </row>
     <row r="32" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="44"/>
-      <c r="M32" s="44"/>
-      <c r="N32" s="44"/>
-      <c r="O32" s="44"/>
-      <c r="P32" s="44"/>
-      <c r="Q32" s="44"/>
-      <c r="R32" s="44"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="69"/>
+      <c r="R32" s="69"/>
     </row>
     <row r="33" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="18"/>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="19"/>
-      <c r="Q33" s="19"/>
-      <c r="R33" s="19"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="44"/>
+      <c r="M33" s="44"/>
+      <c r="N33" s="44"/>
+      <c r="O33" s="44"/>
+      <c r="P33" s="44"/>
+      <c r="Q33" s="44"/>
+      <c r="R33" s="44"/>
     </row>
     <row r="34" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="18"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="44"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="44"/>
+      <c r="O34" s="44"/>
+      <c r="P34" s="44"/>
+      <c r="Q34" s="44"/>
+      <c r="R34" s="44"/>
     </row>
     <row r="35" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
     </row>
     <row r="36" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
     </row>
     <row r="37" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
-      <c r="O37" s="1"/>
-      <c r="P37" s="1"/>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1"/>
     </row>
     <row r="38" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
     </row>
     <row r="39" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
@@ -3070,7 +3103,7 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3090,7 +3123,7 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="61" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -21930,14 +21963,57 @@
       <c r="Q1002" s="1"/>
       <c r="R1002" s="1"/>
     </row>
-    <row r="1003" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1003" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1003" s="1"/>
-    </row>
-    <row r="1004" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1003" s="1"/>
+      <c r="C1003" s="1"/>
+      <c r="D1003" s="1"/>
+      <c r="E1003" s="1"/>
+      <c r="F1003" s="1"/>
+      <c r="G1003" s="1"/>
+      <c r="H1003" s="1"/>
+      <c r="I1003" s="1"/>
+      <c r="J1003" s="1"/>
+      <c r="K1003" s="1"/>
+      <c r="L1003" s="1"/>
+      <c r="M1003" s="1"/>
+      <c r="N1003" s="1"/>
+      <c r="O1003" s="1"/>
+      <c r="P1003" s="1"/>
+      <c r="Q1003" s="1"/>
+      <c r="R1003" s="1"/>
+    </row>
+    <row r="1004" spans="1:18" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1004" s="1"/>
+      <c r="B1004" s="1"/>
+      <c r="C1004" s="1"/>
+      <c r="D1004" s="1"/>
+      <c r="E1004" s="1"/>
+      <c r="F1004" s="1"/>
+      <c r="G1004" s="1"/>
+      <c r="H1004" s="1"/>
+      <c r="I1004" s="1"/>
+      <c r="J1004" s="1"/>
+      <c r="K1004" s="1"/>
+      <c r="L1004" s="1"/>
+      <c r="M1004" s="1"/>
+      <c r="N1004" s="1"/>
+      <c r="O1004" s="1"/>
+      <c r="P1004" s="1"/>
+      <c r="Q1004" s="1"/>
+      <c r="R1004" s="1"/>
+    </row>
+    <row r="1005" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1005" s="1"/>
+    </row>
+    <row r="1006" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1006" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="H3:I3"/>
@@ -21946,9 +22022,6 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <conditionalFormatting sqref="A12:H14 K12:XFD14">
     <cfRule type="colorScale" priority="2">
@@ -21995,11 +22068,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:92" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -22091,11 +22164,11 @@
       <c r="CN1" s="1"/>
     </row>
     <row r="2" spans="1:92" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
-        <v>18</v>
+      <c r="A2" s="103" t="s">
+        <v>17</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -22187,11 +22260,11 @@
       <c r="CN2" s="1"/>
     </row>
     <row r="3" spans="1:92" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
-        <v>19</v>
+      <c r="A3" s="103" t="s">
+        <v>18</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -22284,7 +22357,7 @@
     </row>
     <row r="4" spans="1:92" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
@@ -22379,11 +22452,11 @@
       <c r="CN4" s="1"/>
     </row>
     <row r="5" spans="1:92" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
-        <v>21</v>
+      <c r="A5" s="103" t="s">
+        <v>20</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="103"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -22569,115 +22642,115 @@
       <c r="CN6" s="1"/>
     </row>
     <row r="7" spans="1:92" ht="22.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="106" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="72" t="s">
+      <c r="C7" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="97" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+      <c r="L7" s="98"/>
+      <c r="M7" s="98"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="98"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="98"/>
+      <c r="R7" s="98"/>
+      <c r="S7" s="98"/>
+      <c r="T7" s="98"/>
+      <c r="U7" s="98"/>
+      <c r="V7" s="98"/>
+      <c r="W7" s="98"/>
+      <c r="X7" s="98"/>
+      <c r="Y7" s="98"/>
+      <c r="Z7" s="98"/>
+      <c r="AA7" s="98"/>
+      <c r="AB7" s="98"/>
+      <c r="AC7" s="98"/>
+      <c r="AD7" s="98"/>
+      <c r="AE7" s="98"/>
+      <c r="AF7" s="98"/>
+      <c r="AG7" s="98"/>
+      <c r="AH7" s="99"/>
+      <c r="AI7" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="64"/>
-      <c r="S7" s="64"/>
-      <c r="T7" s="64"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="64"/>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="64"/>
-      <c r="AC7" s="64"/>
-      <c r="AD7" s="64"/>
-      <c r="AE7" s="64"/>
-      <c r="AF7" s="64"/>
-      <c r="AG7" s="64"/>
-      <c r="AH7" s="65"/>
-      <c r="AI7" s="66" t="s">
+      <c r="AJ7" s="98"/>
+      <c r="AK7" s="98"/>
+      <c r="AL7" s="98"/>
+      <c r="AM7" s="98"/>
+      <c r="AN7" s="98"/>
+      <c r="AO7" s="98"/>
+      <c r="AP7" s="98"/>
+      <c r="AQ7" s="98"/>
+      <c r="AR7" s="98"/>
+      <c r="AS7" s="98"/>
+      <c r="AT7" s="98"/>
+      <c r="AU7" s="98"/>
+      <c r="AV7" s="98"/>
+      <c r="AW7" s="98"/>
+      <c r="AX7" s="98"/>
+      <c r="AY7" s="98"/>
+      <c r="AZ7" s="98"/>
+      <c r="BA7" s="98"/>
+      <c r="BB7" s="98"/>
+      <c r="BC7" s="98"/>
+      <c r="BD7" s="98"/>
+      <c r="BE7" s="98"/>
+      <c r="BF7" s="98"/>
+      <c r="BG7" s="98"/>
+      <c r="BH7" s="98"/>
+      <c r="BI7" s="98"/>
+      <c r="BJ7" s="99"/>
+      <c r="BK7" s="100" t="s">
         <v>23</v>
       </c>
-      <c r="AJ7" s="64"/>
-      <c r="AK7" s="64"/>
-      <c r="AL7" s="64"/>
-      <c r="AM7" s="64"/>
-      <c r="AN7" s="64"/>
-      <c r="AO7" s="64"/>
-      <c r="AP7" s="64"/>
-      <c r="AQ7" s="64"/>
-      <c r="AR7" s="64"/>
-      <c r="AS7" s="64"/>
-      <c r="AT7" s="64"/>
-      <c r="AU7" s="64"/>
-      <c r="AV7" s="64"/>
-      <c r="AW7" s="64"/>
-      <c r="AX7" s="64"/>
-      <c r="AY7" s="64"/>
-      <c r="AZ7" s="64"/>
-      <c r="BA7" s="64"/>
-      <c r="BB7" s="64"/>
-      <c r="BC7" s="64"/>
-      <c r="BD7" s="64"/>
-      <c r="BE7" s="64"/>
-      <c r="BF7" s="64"/>
-      <c r="BG7" s="64"/>
-      <c r="BH7" s="64"/>
-      <c r="BI7" s="64"/>
-      <c r="BJ7" s="65"/>
-      <c r="BK7" s="66" t="s">
-        <v>24</v>
-      </c>
-      <c r="BL7" s="64"/>
-      <c r="BM7" s="64"/>
-      <c r="BN7" s="64"/>
-      <c r="BO7" s="64"/>
-      <c r="BP7" s="64"/>
-      <c r="BQ7" s="64"/>
-      <c r="BR7" s="64"/>
-      <c r="BS7" s="64"/>
-      <c r="BT7" s="64"/>
-      <c r="BU7" s="64"/>
-      <c r="BV7" s="64"/>
-      <c r="BW7" s="64"/>
-      <c r="BX7" s="64"/>
-      <c r="BY7" s="64"/>
-      <c r="BZ7" s="64"/>
-      <c r="CA7" s="64"/>
-      <c r="CB7" s="64"/>
-      <c r="CC7" s="64"/>
-      <c r="CD7" s="64"/>
-      <c r="CE7" s="64"/>
-      <c r="CF7" s="64"/>
-      <c r="CG7" s="64"/>
-      <c r="CH7" s="64"/>
-      <c r="CI7" s="64"/>
-      <c r="CJ7" s="64"/>
-      <c r="CK7" s="64"/>
-      <c r="CL7" s="64"/>
-      <c r="CM7" s="64"/>
-      <c r="CN7" s="67"/>
+      <c r="BL7" s="98"/>
+      <c r="BM7" s="98"/>
+      <c r="BN7" s="98"/>
+      <c r="BO7" s="98"/>
+      <c r="BP7" s="98"/>
+      <c r="BQ7" s="98"/>
+      <c r="BR7" s="98"/>
+      <c r="BS7" s="98"/>
+      <c r="BT7" s="98"/>
+      <c r="BU7" s="98"/>
+      <c r="BV7" s="98"/>
+      <c r="BW7" s="98"/>
+      <c r="BX7" s="98"/>
+      <c r="BY7" s="98"/>
+      <c r="BZ7" s="98"/>
+      <c r="CA7" s="98"/>
+      <c r="CB7" s="98"/>
+      <c r="CC7" s="98"/>
+      <c r="CD7" s="98"/>
+      <c r="CE7" s="98"/>
+      <c r="CF7" s="98"/>
+      <c r="CG7" s="98"/>
+      <c r="CH7" s="98"/>
+      <c r="CI7" s="98"/>
+      <c r="CJ7" s="98"/>
+      <c r="CK7" s="98"/>
+      <c r="CL7" s="98"/>
+      <c r="CM7" s="98"/>
+      <c r="CN7" s="101"/>
     </row>
     <row r="8" spans="1:92" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="69"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="73"/>
+      <c r="A8" s="105"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="109"/>
       <c r="D8" s="5">
         <v>1</v>
       </c>
@@ -23016,8 +23089,8 @@
       <c r="BO9" s="21"/>
       <c r="BP9" s="21"/>
       <c r="BQ9" s="21"/>
-      <c r="BR9" s="56" t="s">
-        <v>25</v>
+      <c r="BR9" s="94" t="s">
+        <v>24</v>
       </c>
       <c r="BS9" s="21"/>
       <c r="BT9" s="21"/>
@@ -23112,7 +23185,7 @@
       <c r="BO10" s="26"/>
       <c r="BP10" s="26"/>
       <c r="BQ10" s="26"/>
-      <c r="BR10" s="57"/>
+      <c r="BR10" s="95"/>
       <c r="BS10" s="26"/>
       <c r="BT10" s="26"/>
       <c r="BU10" s="26"/>
@@ -23140,7 +23213,7 @@
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="26"/>
@@ -23208,7 +23281,7 @@
       <c r="BO11" s="26"/>
       <c r="BP11" s="26"/>
       <c r="BQ11" s="26"/>
-      <c r="BR11" s="57"/>
+      <c r="BR11" s="95"/>
       <c r="BS11" s="26"/>
       <c r="BT11" s="26"/>
       <c r="BU11" s="26"/>
@@ -23302,7 +23375,7 @@
       <c r="BO12" s="26"/>
       <c r="BP12" s="26"/>
       <c r="BQ12" s="26"/>
-      <c r="BR12" s="57"/>
+      <c r="BR12" s="95"/>
       <c r="BS12" s="26"/>
       <c r="BT12" s="26"/>
       <c r="BU12" s="26"/>
@@ -23396,7 +23469,7 @@
       <c r="BO13" s="31"/>
       <c r="BP13" s="31"/>
       <c r="BQ13" s="31"/>
-      <c r="BR13" s="57"/>
+      <c r="BR13" s="95"/>
       <c r="BS13" s="31"/>
       <c r="BT13" s="31"/>
       <c r="BU13" s="31"/>
@@ -23490,7 +23563,7 @@
       <c r="BO14" s="21"/>
       <c r="BP14" s="21"/>
       <c r="BQ14" s="21"/>
-      <c r="BR14" s="57"/>
+      <c r="BR14" s="95"/>
       <c r="BS14" s="21"/>
       <c r="BT14" s="21"/>
       <c r="BU14" s="21"/>
@@ -23584,7 +23657,7 @@
       <c r="BO15" s="26"/>
       <c r="BP15" s="26"/>
       <c r="BQ15" s="26"/>
-      <c r="BR15" s="57"/>
+      <c r="BR15" s="95"/>
       <c r="BS15" s="26"/>
       <c r="BT15" s="26"/>
       <c r="BU15" s="26"/>
@@ -23678,7 +23751,7 @@
       <c r="BO16" s="26"/>
       <c r="BP16" s="26"/>
       <c r="BQ16" s="26"/>
-      <c r="BR16" s="57"/>
+      <c r="BR16" s="95"/>
       <c r="BS16" s="26"/>
       <c r="BT16" s="26"/>
       <c r="BU16" s="26"/>
@@ -23706,7 +23779,7 @@
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="26"/>
@@ -23774,7 +23847,7 @@
       <c r="BO17" s="26"/>
       <c r="BP17" s="26"/>
       <c r="BQ17" s="26"/>
-      <c r="BR17" s="57"/>
+      <c r="BR17" s="95"/>
       <c r="BS17" s="26"/>
       <c r="BT17" s="26"/>
       <c r="BU17" s="26"/>
@@ -23868,7 +23941,7 @@
       <c r="BO18" s="31"/>
       <c r="BP18" s="31"/>
       <c r="BQ18" s="31"/>
-      <c r="BR18" s="57"/>
+      <c r="BR18" s="95"/>
       <c r="BS18" s="31"/>
       <c r="BT18" s="31"/>
       <c r="BU18" s="31"/>
@@ -23962,7 +24035,7 @@
       <c r="BO19" s="21"/>
       <c r="BP19" s="21"/>
       <c r="BQ19" s="21"/>
-      <c r="BR19" s="57"/>
+      <c r="BR19" s="95"/>
       <c r="BS19" s="21"/>
       <c r="BT19" s="21"/>
       <c r="BU19" s="21"/>
@@ -23990,7 +24063,7 @@
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="25"/>
       <c r="E20" s="26"/>
@@ -24058,7 +24131,7 @@
       <c r="BO20" s="26"/>
       <c r="BP20" s="26"/>
       <c r="BQ20" s="26"/>
-      <c r="BR20" s="57"/>
+      <c r="BR20" s="95"/>
       <c r="BS20" s="26"/>
       <c r="BT20" s="26"/>
       <c r="BU20" s="26"/>
@@ -24152,7 +24225,7 @@
       <c r="BO21" s="26"/>
       <c r="BP21" s="26"/>
       <c r="BQ21" s="26"/>
-      <c r="BR21" s="57"/>
+      <c r="BR21" s="95"/>
       <c r="BS21" s="26"/>
       <c r="BT21" s="26"/>
       <c r="BU21" s="26"/>
@@ -24246,7 +24319,7 @@
       <c r="BO22" s="26"/>
       <c r="BP22" s="26"/>
       <c r="BQ22" s="26"/>
-      <c r="BR22" s="57"/>
+      <c r="BR22" s="95"/>
       <c r="BS22" s="26"/>
       <c r="BT22" s="26"/>
       <c r="BU22" s="26"/>
@@ -24340,7 +24413,7 @@
       <c r="BO23" s="31"/>
       <c r="BP23" s="31"/>
       <c r="BQ23" s="31"/>
-      <c r="BR23" s="57"/>
+      <c r="BR23" s="95"/>
       <c r="BS23" s="31"/>
       <c r="BT23" s="31"/>
       <c r="BU23" s="31"/>
@@ -24434,7 +24507,7 @@
       <c r="BO24" s="21"/>
       <c r="BP24" s="21"/>
       <c r="BQ24" s="21"/>
-      <c r="BR24" s="57"/>
+      <c r="BR24" s="95"/>
       <c r="BS24" s="21"/>
       <c r="BT24" s="21"/>
       <c r="BU24" s="21"/>
@@ -24528,7 +24601,7 @@
       <c r="BO25" s="26"/>
       <c r="BP25" s="26"/>
       <c r="BQ25" s="26"/>
-      <c r="BR25" s="57"/>
+      <c r="BR25" s="95"/>
       <c r="BS25" s="26"/>
       <c r="BT25" s="26"/>
       <c r="BU25" s="26"/>
@@ -24622,7 +24695,7 @@
       <c r="BO26" s="26"/>
       <c r="BP26" s="26"/>
       <c r="BQ26" s="26"/>
-      <c r="BR26" s="57"/>
+      <c r="BR26" s="95"/>
       <c r="BS26" s="26"/>
       <c r="BT26" s="26"/>
       <c r="BU26" s="26"/>
@@ -24650,7 +24723,7 @@
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
       <c r="C27" s="36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="26"/>
@@ -24718,7 +24791,7 @@
       <c r="BO27" s="26"/>
       <c r="BP27" s="26"/>
       <c r="BQ27" s="26"/>
-      <c r="BR27" s="57"/>
+      <c r="BR27" s="95"/>
       <c r="BS27" s="26"/>
       <c r="BT27" s="26"/>
       <c r="BU27" s="26"/>
@@ -24812,7 +24885,7 @@
       <c r="BO28" s="31"/>
       <c r="BP28" s="31"/>
       <c r="BQ28" s="31"/>
-      <c r="BR28" s="58"/>
+      <c r="BR28" s="96"/>
       <c r="BS28" s="31"/>
       <c r="BT28" s="31"/>
       <c r="BU28" s="31"/>
@@ -25625,9 +25698,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -25769,19 +25845,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B054B1D-A094-48ED-88FD-A6F94F085238}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2FCB554-154D-4A5E-B8F9-F654C19424B8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25805,9 +25877,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2FCB554-154D-4A5E-B8F9-F654C19424B8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B054B1D-A094-48ED-88FD-A6F94F085238}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>